<commit_message>
Update the Summary.R and the related files.
</commit_message>
<xml_diff>
--- a/demo/Analysis_Results/OutputFiles/Summary.xlsx
+++ b/demo/Analysis_Results/OutputFiles/Summary.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="177">
   <si>
     <t xml:space="preserve">primer_index</t>
   </si>
@@ -166,7 +166,7 @@
     <t xml:space="preserve">./aaAlignment/set191_1_aa_align_muscle.html</t>
   </si>
   <si>
-    <t xml:space="preserve">AATGGCTGAATCTTTCTTAAGCAAAAGACATCTTCAACTACAACTACTACTACAACTTCTATTGACGCCGATAATAATAATTCTTCTAATTCTACTACTCCTGTTGTGAAAACCACCAAGACTAAGAGAACTAGAAAGTCTGTTGATTCTTTTGGACAAAGAACTTCTCAATATAGGGGAGTTACTAGACATAGATGGACTGGAAGATATGAAGCTCATCTTTGGGATAATTCTTGTAAGAAGGAAGGACAAACTAGGAAGGGAAGGCAAGGAGGATATGATGATGAACAAAAGGCTGCTCGAGCTTATGATCTTGCTGCTCTTAAGTATTGGGGACCTACTACTCATCTTAATTTTCCTCTTTCTAATTACGAAAAGGAACGAGGAACTGGAAGAACATGAATAGACAAGAATTTGTTGCTATGCTTAGAAGAAAGTCTACTGGGTTTTCTAGGGGAGCTTCTAATTATAGAGGAGTTACAAGACATCATCAACATGGAAGATGGCAAGCTAGAATTGGAAGAGTTGCTGGAAATAAGGATCTTTATCTTGGAACTTATGTTACTCCGATGCATGTTATGCAACTTCATAAGAAGAAGCAAAGACTTCATATGACTTGGCAACAATGA</t>
+    <t xml:space="preserve">AATGGCTGAATCTTTCTTAAGCAAAAGACATCTTCAACTACAACTACTACTACAACTTCTATTGACGCCGATAATAATAATTCTTCTAATTCTACTACTCCTGTTGTGAAAACCACCAAGACTAAGAGAACTAGAAAGTCTGTTGATTCTTTTGGACAAAGAACTTCTCAATATAGGGGAGTTACTAGACATAGATGGACTGGAAGATATGAAGCTCATCTTTGGGATAATTCTTGTAAGAAGGAAGGACAAACTAGGAAGGGAAGGCAAGGAGGATATGATGATGAACAAAAGGCTGCTCGAGCTTATGATCTTGCTGCTCTTAAGTATTGGGGACCTACTACTCATCTTAATTTTCCTCTTTCTAATTACGAAAAGGAATGAGGAAATGCAAGAACATGAATAGACAAGAATTTGTTGCTATGCTTAGAAGAAATTCTACTGGGTTTTCTAGGGGAGCTTCTAATTATAGAGGAGTTACAAGACATCATCAACATGGAAGATGGCAAGCTAGAATTGGAAGAGTTGCTGGAAATAAGGATCTTTATCTTGGAACTTATGTTACTCCGATGCATGTTATGCAACTTCATAAGAAGAAGCAAAGACTTCATATGACTTGGCAACAATGA</t>
   </si>
   <si>
     <t xml:space="preserve">set191_2</t>
@@ -367,24 +367,6 @@
     <t xml:space="preserve">Pro_Identity_pct_racon_3rd</t>
   </si>
   <si>
-    <t xml:space="preserve">RefORFlength_sam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RefORFlength_draft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RefORFlength_racon_1rd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RefORFlength_racon_2rd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RefORFlength_racon_3rd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RefORFlength_medaka_1rd</t>
-  </si>
-  <si>
     <t xml:space="preserve">ORFlength_sam</t>
   </si>
   <si>
@@ -466,6 +448,9 @@
     <t xml:space="preserve">missenseMutation_racon_3rd</t>
   </si>
   <si>
+    <t xml:space="preserve">RefORFlength</t>
+  </si>
+  <si>
     <t xml:space="preserve">AssembledDNALength</t>
   </si>
   <si>
@@ -478,10 +463,16 @@
     <t xml:space="preserve">561/643</t>
   </si>
   <si>
-    <t xml:space="preserve">549/657</t>
-  </si>
-  <si>
-    <t xml:space="preserve">558/652</t>
+    <t xml:space="preserve">550/655</t>
+  </si>
+  <si>
+    <t xml:space="preserve">559/653</t>
+  </si>
+  <si>
+    <t xml:space="preserve">560/654</t>
+  </si>
+  <si>
+    <t xml:space="preserve">557/652</t>
   </si>
   <si>
     <t xml:space="preserve">5/229</t>
@@ -503,6 +494,9 @@
   </si>
   <si>
     <t xml:space="preserve">643/646</t>
+  </si>
+  <si>
+    <t xml:space="preserve">643/647</t>
   </si>
   <si>
     <t xml:space="preserve">643/643</t>
@@ -977,7 +971,7 @@
         <v>643</v>
       </c>
       <c r="G2" t="n">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H2" t="n">
         <v>74</v>
@@ -1163,7 +1157,7 @@
       </c>
       <c r="N2"/>
       <c r="O2" t="n">
-        <v>85.6</v>
+        <v>85.4</v>
       </c>
       <c r="P2" t="s">
         <v>45</v>
@@ -1216,7 +1210,7 @@
         <v>643</v>
       </c>
       <c r="F3" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G3" t="n">
         <v>65</v>
@@ -1292,7 +1286,7 @@
         <v>643</v>
       </c>
       <c r="F4" t="n">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G4" t="n">
         <v>74</v>
@@ -1442,13 +1436,13 @@
         <v>643</v>
       </c>
       <c r="F6" t="n">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="G6" t="n">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="H6" t="n">
-        <v>1064.49</v>
+        <v>1063.64</v>
       </c>
       <c r="I6"/>
       <c r="J6" t="s">
@@ -1523,10 +1517,10 @@
         <v>428</v>
       </c>
       <c r="G7" t="n">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="H7" t="n">
-        <v>353.988</v>
+        <v>355.776</v>
       </c>
       <c r="I7"/>
       <c r="J7" t="s">
@@ -1810,25 +1804,25 @@
         <v>127</v>
       </c>
       <c r="BH1" t="s">
+        <v>40</v>
+      </c>
+      <c r="BI1" t="s">
         <v>128</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BJ1" t="s">
         <v>129</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BK1" t="s">
         <v>130</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BL1" t="s">
         <v>131</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BM1" t="s">
         <v>132</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BN1" t="s">
         <v>133</v>
-      </c>
-      <c r="BN1" t="s">
-        <v>40</v>
       </c>
       <c r="BO1" t="s">
         <v>134</v>
@@ -1846,87 +1840,72 @@
         <v>138</v>
       </c>
       <c r="BT1" t="s">
+        <v>39</v>
+      </c>
+      <c r="BU1" t="s">
         <v>139</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="BV1" t="s">
         <v>140</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="BW1" t="s">
         <v>141</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="BX1" t="s">
         <v>142</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="BY1" t="s">
         <v>143</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="BZ1" t="s">
+        <v>12</v>
+      </c>
+      <c r="CA1" t="s">
         <v>144</v>
       </c>
-      <c r="BZ1" t="s">
-        <v>39</v>
-      </c>
-      <c r="CA1" t="s">
+      <c r="CB1" t="s">
+        <v>13</v>
+      </c>
+      <c r="CC1" t="s">
+        <v>9</v>
+      </c>
+      <c r="CD1" t="s">
+        <v>14</v>
+      </c>
+      <c r="CE1" t="s">
+        <v>15</v>
+      </c>
+      <c r="CF1" t="s">
+        <v>16</v>
+      </c>
+      <c r="CG1" t="s">
+        <v>17</v>
+      </c>
+      <c r="CH1" t="s">
+        <v>18</v>
+      </c>
+      <c r="CI1" t="s">
+        <v>19</v>
+      </c>
+      <c r="CJ1" t="s">
         <v>145</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="CK1" t="s">
+        <v>20</v>
+      </c>
+      <c r="CL1" t="s">
         <v>146</v>
       </c>
-      <c r="CC1" t="s">
-        <v>147</v>
-      </c>
-      <c r="CD1" t="s">
-        <v>148</v>
-      </c>
-      <c r="CE1" t="s">
-        <v>149</v>
-      </c>
-      <c r="CF1" t="s">
-        <v>12</v>
-      </c>
-      <c r="CG1" t="s">
-        <v>13</v>
-      </c>
-      <c r="CH1" t="s">
-        <v>9</v>
-      </c>
-      <c r="CI1" t="s">
-        <v>14</v>
-      </c>
-      <c r="CJ1" t="s">
-        <v>15</v>
-      </c>
-      <c r="CK1" t="s">
-        <v>16</v>
-      </c>
-      <c r="CL1" t="s">
-        <v>17</v>
-      </c>
       <c r="CM1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="CN1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="CO1" t="s">
-        <v>150</v>
+        <v>10</v>
       </c>
       <c r="CP1" t="s">
-        <v>20</v>
-      </c>
-      <c r="CQ1" t="s">
-        <v>151</v>
-      </c>
-      <c r="CR1" t="s">
-        <v>21</v>
-      </c>
-      <c r="CS1" t="s">
-        <v>11</v>
-      </c>
-      <c r="CT1" t="s">
-        <v>10</v>
-      </c>
-      <c r="CU1" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1965,22 +1944,22 @@
         <v>643</v>
       </c>
       <c r="L2" t="s">
+        <v>147</v>
+      </c>
+      <c r="M2" t="s">
+        <v>148</v>
+      </c>
+      <c r="N2" t="s">
+        <v>149</v>
+      </c>
+      <c r="O2" t="s">
+        <v>150</v>
+      </c>
+      <c r="P2" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q2" t="s">
         <v>152</v>
-      </c>
-      <c r="M2" t="s">
-        <v>153</v>
-      </c>
-      <c r="N2" t="s">
-        <v>154</v>
-      </c>
-      <c r="O2" t="s">
-        <v>155</v>
-      </c>
-      <c r="P2" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>155</v>
       </c>
       <c r="R2" t="n">
         <v>87.7</v>
@@ -1989,7 +1968,7 @@
         <v>87.2</v>
       </c>
       <c r="T2" t="n">
-        <v>83.6</v>
+        <v>84</v>
       </c>
       <c r="U2" t="n">
         <v>85.6</v>
@@ -1998,7 +1977,7 @@
         <v>85.6</v>
       </c>
       <c r="W2" t="n">
-        <v>85.6</v>
+        <v>85.4</v>
       </c>
       <c r="X2" t="n">
         <v>643</v>
@@ -2007,13 +1986,13 @@
         <v>643</v>
       </c>
       <c r="Z2" t="n">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="AA2" t="n">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="AB2" t="n">
-        <v>652</v>
+        <v>654</v>
       </c>
       <c r="AC2" t="n">
         <v>652</v>
@@ -2026,22 +2005,22 @@
       <c r="AI2"/>
       <c r="AJ2"/>
       <c r="AK2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="AL2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="AM2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="AN2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="AO2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="AP2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="AQ2" t="n">
         <v>2.2</v>
@@ -2062,41 +2041,29 @@
         <v>2.2</v>
       </c>
       <c r="AW2" t="n">
-        <v>213</v>
+        <v>32</v>
       </c>
       <c r="AX2" t="n">
-        <v>213</v>
+        <v>31</v>
       </c>
       <c r="AY2" t="n">
-        <v>213</v>
+        <v>35</v>
       </c>
       <c r="AZ2" t="n">
-        <v>213</v>
+        <v>35</v>
       </c>
       <c r="BA2" t="n">
-        <v>213</v>
+        <v>35</v>
       </c>
       <c r="BB2" t="n">
-        <v>213</v>
-      </c>
-      <c r="BC2" t="n">
-        <v>32</v>
-      </c>
-      <c r="BD2" t="n">
-        <v>31</v>
-      </c>
-      <c r="BE2" t="n">
         <v>35</v>
       </c>
-      <c r="BF2" t="n">
-        <v>35</v>
-      </c>
-      <c r="BG2" t="n">
-        <v>35</v>
-      </c>
-      <c r="BH2" t="n">
-        <v>35</v>
-      </c>
+      <c r="BC2"/>
+      <c r="BD2"/>
+      <c r="BE2"/>
+      <c r="BF2"/>
+      <c r="BG2"/>
+      <c r="BH2"/>
       <c r="BI2"/>
       <c r="BJ2"/>
       <c r="BK2"/>
@@ -2105,69 +2072,66 @@
       <c r="BN2"/>
       <c r="BO2"/>
       <c r="BP2"/>
-      <c r="BQ2"/>
-      <c r="BR2"/>
-      <c r="BS2"/>
-      <c r="BT2"/>
+      <c r="BQ2" t="s">
+        <v>45</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>45</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>45</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>45</v>
+      </c>
       <c r="BU2"/>
       <c r="BV2"/>
-      <c r="BW2" t="s">
-        <v>45</v>
-      </c>
-      <c r="BX2" t="s">
-        <v>45</v>
-      </c>
-      <c r="BY2" t="s">
-        <v>45</v>
-      </c>
-      <c r="BZ2" t="s">
-        <v>45</v>
-      </c>
-      <c r="CA2"/>
+      <c r="BW2"/>
+      <c r="BX2"/>
+      <c r="BY2"/>
+      <c r="BZ2"/>
+      <c r="CA2" t="n">
+        <v>213</v>
+      </c>
       <c r="CB2"/>
       <c r="CC2"/>
-      <c r="CD2"/>
-      <c r="CE2"/>
-      <c r="CF2"/>
-      <c r="CG2"/>
-      <c r="CH2"/>
+      <c r="CD2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="CE2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="CF2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="CG2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="CH2" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="CI2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="CJ2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="CK2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="CL2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="CM2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="CN2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="CO2" t="n">
+      <c r="CJ2" t="n">
         <v>629</v>
       </c>
+      <c r="CK2" t="s">
+        <v>50</v>
+      </c>
+      <c r="CL2" t="s">
+        <v>155</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>33</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>26</v>
+      </c>
+      <c r="CO2" t="s">
+        <v>43</v>
+      </c>
       <c r="CP2" t="s">
-        <v>50</v>
-      </c>
-      <c r="CQ2" t="s">
-        <v>158</v>
-      </c>
-      <c r="CR2" t="s">
-        <v>33</v>
-      </c>
-      <c r="CS2" t="s">
-        <v>26</v>
-      </c>
-      <c r="CT2" t="s">
-        <v>43</v>
-      </c>
-      <c r="CU2" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2185,7 +2149,7 @@
         <v>4</v>
       </c>
       <c r="E3" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F3" t="n">
         <v>65</v>
@@ -2206,22 +2170,22 @@
         <v>643</v>
       </c>
       <c r="L3" t="s">
+        <v>156</v>
+      </c>
+      <c r="M3" t="s">
+        <v>157</v>
+      </c>
+      <c r="N3" t="s">
+        <v>158</v>
+      </c>
+      <c r="O3" t="s">
         <v>159</v>
       </c>
-      <c r="M3" t="s">
+      <c r="P3" t="s">
         <v>160</v>
       </c>
-      <c r="N3" t="s">
+      <c r="Q3" t="s">
         <v>161</v>
-      </c>
-      <c r="O3" t="s">
-        <v>162</v>
-      </c>
-      <c r="P3" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>163</v>
       </c>
       <c r="R3" t="n">
         <v>99.7</v>
@@ -2236,7 +2200,7 @@
         <v>99.5</v>
       </c>
       <c r="V3" t="n">
-        <v>99.5</v>
+        <v>99.4</v>
       </c>
       <c r="W3" t="n">
         <v>100</v>
@@ -2254,7 +2218,7 @@
         <v>646</v>
       </c>
       <c r="AB3" t="n">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="AC3" t="n">
         <v>643</v>
@@ -2271,22 +2235,22 @@
         <v>53</v>
       </c>
       <c r="AK3" t="s">
+        <v>162</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>162</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>163</v>
+      </c>
+      <c r="AN3" t="s">
         <v>164</v>
       </c>
-      <c r="AL3" t="s">
-        <v>164</v>
-      </c>
-      <c r="AM3" t="s">
+      <c r="AO3" t="s">
+        <v>163</v>
+      </c>
+      <c r="AP3" t="s">
         <v>165</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>166</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>166</v>
-      </c>
-      <c r="AP3" t="s">
-        <v>167</v>
       </c>
       <c r="AQ3" t="n">
         <v>60.3</v>
@@ -2301,46 +2265,36 @@
         <v>99.5</v>
       </c>
       <c r="AU3" t="n">
-        <v>99.5</v>
+        <v>77.9</v>
       </c>
       <c r="AV3" t="n">
         <v>100</v>
       </c>
       <c r="AW3" t="n">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="AX3" t="n">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="AY3" t="n">
-        <v>213</v>
+        <v>169</v>
       </c>
       <c r="AZ3" t="n">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="BA3" t="n">
-        <v>213</v>
+        <v>170</v>
       </c>
       <c r="BB3" t="n">
         <v>213</v>
       </c>
-      <c r="BC3" t="n">
-        <v>208</v>
-      </c>
-      <c r="BD3" t="n">
-        <v>208</v>
-      </c>
-      <c r="BE3" t="n">
-        <v>169</v>
-      </c>
-      <c r="BF3" t="n">
-        <v>214</v>
-      </c>
-      <c r="BG3" t="n">
-        <v>214</v>
-      </c>
-      <c r="BH3" t="n">
-        <v>213</v>
+      <c r="BC3"/>
+      <c r="BD3"/>
+      <c r="BE3"/>
+      <c r="BF3"/>
+      <c r="BG3"/>
+      <c r="BH3" t="s">
+        <v>53</v>
       </c>
       <c r="BI3"/>
       <c r="BJ3"/>
@@ -2352,67 +2306,62 @@
       </c>
       <c r="BO3"/>
       <c r="BP3"/>
-      <c r="BQ3"/>
-      <c r="BR3"/>
-      <c r="BS3"/>
-      <c r="BT3" t="s">
-        <v>53</v>
-      </c>
+      <c r="BQ3" t="s">
+        <v>60</v>
+      </c>
+      <c r="BR3" t="s">
+        <v>60</v>
+      </c>
+      <c r="BS3" t="s">
+        <v>60</v>
+      </c>
+      <c r="BT3"/>
       <c r="BU3"/>
       <c r="BV3"/>
-      <c r="BW3" t="s">
-        <v>60</v>
-      </c>
-      <c r="BX3" t="s">
-        <v>60</v>
-      </c>
-      <c r="BY3" t="s">
-        <v>60</v>
-      </c>
+      <c r="BW3"/>
+      <c r="BX3"/>
+      <c r="BY3"/>
       <c r="BZ3"/>
-      <c r="CA3"/>
+      <c r="CA3" t="n">
+        <v>213</v>
+      </c>
       <c r="CB3"/>
       <c r="CC3"/>
-      <c r="CD3"/>
-      <c r="CE3"/>
-      <c r="CF3"/>
-      <c r="CG3"/>
-      <c r="CH3"/>
+      <c r="CD3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="CE3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="CF3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="CG3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="CH3" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="CI3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="CJ3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="CK3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="CL3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="CM3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="CN3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="CO3" t="n">
-        <v>643</v>
+      <c r="CJ3" t="n">
+        <v>643</v>
+      </c>
+      <c r="CK3" t="s">
+        <v>33</v>
+      </c>
+      <c r="CL3" t="s">
+        <v>166</v>
+      </c>
+      <c r="CM3" t="s">
+        <v>33</v>
+      </c>
+      <c r="CN3"/>
+      <c r="CO3" t="s">
+        <v>52</v>
       </c>
       <c r="CP3" t="s">
-        <v>33</v>
-      </c>
-      <c r="CQ3" t="s">
-        <v>168</v>
-      </c>
-      <c r="CR3" t="s">
-        <v>33</v>
-      </c>
-      <c r="CS3"/>
-      <c r="CT3" t="s">
-        <v>52</v>
-      </c>
-      <c r="CU3" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2430,7 +2379,7 @@
         <v>4</v>
       </c>
       <c r="E4" t="n">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F4" t="n">
         <v>74</v>
@@ -2451,22 +2400,22 @@
         <v>643</v>
       </c>
       <c r="L4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="M4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="N4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="O4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="P4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="Q4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="R4" t="n">
         <v>100</v>
@@ -2526,22 +2475,22 @@
         <v>53</v>
       </c>
       <c r="AK4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AL4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AM4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AN4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AO4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AP4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AQ4" t="n">
         <v>100</v>
@@ -2579,23 +2528,23 @@
       <c r="BB4" t="n">
         <v>213</v>
       </c>
-      <c r="BC4" t="n">
-        <v>213</v>
-      </c>
-      <c r="BD4" t="n">
-        <v>213</v>
-      </c>
-      <c r="BE4" t="n">
-        <v>213</v>
-      </c>
-      <c r="BF4" t="n">
-        <v>213</v>
-      </c>
-      <c r="BG4" t="n">
-        <v>213</v>
-      </c>
-      <c r="BH4" t="n">
-        <v>213</v>
+      <c r="BC4" t="s">
+        <v>53</v>
+      </c>
+      <c r="BD4" t="s">
+        <v>53</v>
+      </c>
+      <c r="BE4" t="s">
+        <v>53</v>
+      </c>
+      <c r="BF4" t="s">
+        <v>53</v>
+      </c>
+      <c r="BG4" t="s">
+        <v>53</v>
+      </c>
+      <c r="BH4" t="s">
+        <v>53</v>
       </c>
       <c r="BI4" t="s">
         <v>53</v>
@@ -2615,73 +2564,58 @@
       <c r="BN4" t="s">
         <v>53</v>
       </c>
-      <c r="BO4" t="s">
-        <v>53</v>
-      </c>
-      <c r="BP4" t="s">
-        <v>53</v>
-      </c>
-      <c r="BQ4" t="s">
-        <v>53</v>
-      </c>
-      <c r="BR4" t="s">
-        <v>53</v>
-      </c>
-      <c r="BS4" t="s">
-        <v>53</v>
-      </c>
-      <c r="BT4" t="s">
-        <v>53</v>
-      </c>
+      <c r="BO4"/>
+      <c r="BP4"/>
+      <c r="BQ4"/>
+      <c r="BR4"/>
+      <c r="BS4"/>
+      <c r="BT4"/>
       <c r="BU4"/>
       <c r="BV4"/>
       <c r="BW4"/>
       <c r="BX4"/>
       <c r="BY4"/>
       <c r="BZ4"/>
-      <c r="CA4"/>
+      <c r="CA4" t="n">
+        <v>213</v>
+      </c>
       <c r="CB4"/>
       <c r="CC4"/>
-      <c r="CD4"/>
-      <c r="CE4"/>
-      <c r="CF4"/>
-      <c r="CG4"/>
-      <c r="CH4"/>
+      <c r="CD4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="CE4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="CF4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="CG4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="CH4" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="CI4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="CJ4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="CK4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="CL4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="CM4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="CN4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="CO4" t="n">
-        <v>643</v>
+      <c r="CJ4" t="n">
+        <v>643</v>
+      </c>
+      <c r="CK4" t="s">
+        <v>33</v>
+      </c>
+      <c r="CL4" t="s">
+        <v>33</v>
+      </c>
+      <c r="CM4" t="s">
+        <v>33</v>
+      </c>
+      <c r="CN4"/>
+      <c r="CO4" t="s">
+        <v>26</v>
       </c>
       <c r="CP4" t="s">
-        <v>33</v>
-      </c>
-      <c r="CQ4" t="s">
-        <v>33</v>
-      </c>
-      <c r="CR4" t="s">
-        <v>33</v>
-      </c>
-      <c r="CS4"/>
-      <c r="CT4" t="s">
-        <v>26</v>
-      </c>
-      <c r="CU4" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2720,22 +2654,22 @@
         <v>643</v>
       </c>
       <c r="L5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="M5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="N5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="O5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="P5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="Q5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="R5" t="n">
         <v>91.7</v>
@@ -2781,22 +2715,22 @@
       <c r="AI5"/>
       <c r="AJ5"/>
       <c r="AK5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="AL5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="AM5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="AN5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="AO5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="AP5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="AQ5" t="n">
         <v>0.9</v>
@@ -2817,41 +2751,29 @@
         <v>0.9</v>
       </c>
       <c r="AW5" t="n">
-        <v>213</v>
+        <v>5</v>
       </c>
       <c r="AX5" t="n">
-        <v>213</v>
+        <v>5</v>
       </c>
       <c r="AY5" t="n">
-        <v>213</v>
+        <v>5</v>
       </c>
       <c r="AZ5" t="n">
-        <v>213</v>
+        <v>5</v>
       </c>
       <c r="BA5" t="n">
-        <v>213</v>
+        <v>5</v>
       </c>
       <c r="BB5" t="n">
-        <v>213</v>
-      </c>
-      <c r="BC5" t="n">
         <v>5</v>
       </c>
-      <c r="BD5" t="n">
-        <v>5</v>
-      </c>
-      <c r="BE5" t="n">
-        <v>5</v>
-      </c>
-      <c r="BF5" t="n">
-        <v>5</v>
-      </c>
-      <c r="BG5" t="n">
-        <v>5</v>
-      </c>
-      <c r="BH5" t="n">
-        <v>5</v>
-      </c>
+      <c r="BC5"/>
+      <c r="BD5"/>
+      <c r="BE5"/>
+      <c r="BF5"/>
+      <c r="BG5"/>
+      <c r="BH5"/>
       <c r="BI5"/>
       <c r="BJ5"/>
       <c r="BK5"/>
@@ -2860,69 +2782,66 @@
       <c r="BN5"/>
       <c r="BO5"/>
       <c r="BP5"/>
-      <c r="BQ5"/>
-      <c r="BR5"/>
-      <c r="BS5"/>
-      <c r="BT5"/>
+      <c r="BQ5" t="s">
+        <v>60</v>
+      </c>
+      <c r="BR5" t="s">
+        <v>60</v>
+      </c>
+      <c r="BS5" t="s">
+        <v>60</v>
+      </c>
+      <c r="BT5" t="s">
+        <v>60</v>
+      </c>
       <c r="BU5"/>
       <c r="BV5"/>
-      <c r="BW5" t="s">
-        <v>60</v>
-      </c>
-      <c r="BX5" t="s">
-        <v>60</v>
-      </c>
-      <c r="BY5" t="s">
-        <v>60</v>
-      </c>
-      <c r="BZ5" t="s">
-        <v>60</v>
-      </c>
-      <c r="CA5"/>
+      <c r="BW5"/>
+      <c r="BX5"/>
+      <c r="BY5"/>
+      <c r="BZ5"/>
+      <c r="CA5" t="n">
+        <v>213</v>
+      </c>
       <c r="CB5"/>
       <c r="CC5"/>
-      <c r="CD5"/>
-      <c r="CE5"/>
-      <c r="CF5"/>
-      <c r="CG5"/>
-      <c r="CH5"/>
+      <c r="CD5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="CE5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="CF5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="CG5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="CH5" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="CI5" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="CJ5" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="CK5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="CL5" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="CM5" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="CN5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="CO5" t="n">
-        <v>643</v>
+      <c r="CJ5" t="n">
+        <v>643</v>
+      </c>
+      <c r="CK5" t="s">
+        <v>65</v>
+      </c>
+      <c r="CL5" t="s">
+        <v>170</v>
+      </c>
+      <c r="CM5" t="s">
+        <v>33</v>
+      </c>
+      <c r="CN5" t="s">
+        <v>26</v>
+      </c>
+      <c r="CO5" t="s">
+        <v>26</v>
       </c>
       <c r="CP5" t="s">
-        <v>65</v>
-      </c>
-      <c r="CQ5" t="s">
-        <v>172</v>
-      </c>
-      <c r="CR5" t="s">
-        <v>33</v>
-      </c>
-      <c r="CS5" t="s">
-        <v>26</v>
-      </c>
-      <c r="CT5" t="s">
-        <v>26</v>
-      </c>
-      <c r="CU5" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2940,16 +2859,16 @@
         <v>4</v>
       </c>
       <c r="E6" t="n">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="F6" t="n">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="G6" t="n">
         <v>100</v>
       </c>
       <c r="H6" t="n">
-        <v>1064.49</v>
+        <v>1063.64</v>
       </c>
       <c r="I6" t="n">
         <v>28</v>
@@ -2961,22 +2880,22 @@
         <v>643</v>
       </c>
       <c r="L6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="M6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="N6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="O6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="P6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="Q6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="R6" t="n">
         <v>99.7</v>
@@ -3024,22 +2943,22 @@
         <v>53</v>
       </c>
       <c r="AK6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AL6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AM6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AN6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AO6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AP6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="AQ6" t="n">
         <v>100</v>
@@ -3077,23 +2996,23 @@
       <c r="BB6" t="n">
         <v>213</v>
       </c>
-      <c r="BC6" t="n">
-        <v>213</v>
-      </c>
-      <c r="BD6" t="n">
-        <v>213</v>
-      </c>
-      <c r="BE6" t="n">
-        <v>213</v>
-      </c>
-      <c r="BF6" t="n">
-        <v>213</v>
-      </c>
-      <c r="BG6" t="n">
-        <v>213</v>
-      </c>
-      <c r="BH6" t="n">
-        <v>213</v>
+      <c r="BC6" t="s">
+        <v>53</v>
+      </c>
+      <c r="BD6" t="s">
+        <v>53</v>
+      </c>
+      <c r="BE6" t="s">
+        <v>53</v>
+      </c>
+      <c r="BF6" t="s">
+        <v>53</v>
+      </c>
+      <c r="BG6" t="s">
+        <v>53</v>
+      </c>
+      <c r="BH6" t="s">
+        <v>53</v>
       </c>
       <c r="BI6" t="s">
         <v>53</v>
@@ -3113,83 +3032,68 @@
       <c r="BN6" t="s">
         <v>53</v>
       </c>
-      <c r="BO6" t="s">
-        <v>53</v>
-      </c>
-      <c r="BP6" t="s">
-        <v>53</v>
-      </c>
+      <c r="BO6"/>
+      <c r="BP6"/>
       <c r="BQ6" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="BR6" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="BS6" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="BT6" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="BU6"/>
       <c r="BV6"/>
-      <c r="BW6" t="s">
-        <v>69</v>
-      </c>
-      <c r="BX6" t="s">
-        <v>69</v>
-      </c>
-      <c r="BY6" t="s">
-        <v>69</v>
-      </c>
-      <c r="BZ6" t="s">
-        <v>69</v>
-      </c>
-      <c r="CA6"/>
+      <c r="BW6"/>
+      <c r="BX6"/>
+      <c r="BY6"/>
+      <c r="BZ6"/>
+      <c r="CA6" t="n">
+        <v>213</v>
+      </c>
       <c r="CB6"/>
       <c r="CC6"/>
-      <c r="CD6"/>
-      <c r="CE6"/>
-      <c r="CF6"/>
-      <c r="CG6"/>
-      <c r="CH6"/>
+      <c r="CD6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="CE6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="CF6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="CG6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="CH6" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="CI6" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="CJ6" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="CK6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="CL6" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="CM6" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="CN6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="CO6" t="n">
-        <v>643</v>
+      <c r="CJ6" t="n">
+        <v>643</v>
+      </c>
+      <c r="CK6" t="s">
+        <v>74</v>
+      </c>
+      <c r="CL6" t="s">
+        <v>172</v>
+      </c>
+      <c r="CM6" t="s">
+        <v>33</v>
+      </c>
+      <c r="CN6" t="s">
+        <v>26</v>
+      </c>
+      <c r="CO6" t="s">
+        <v>67</v>
       </c>
       <c r="CP6" t="s">
-        <v>74</v>
-      </c>
-      <c r="CQ6" t="s">
-        <v>174</v>
-      </c>
-      <c r="CR6" t="s">
-        <v>33</v>
-      </c>
-      <c r="CS6" t="s">
-        <v>26</v>
-      </c>
-      <c r="CT6" t="s">
-        <v>67</v>
-      </c>
-      <c r="CU6" t="s">
         <v>68</v>
       </c>
     </row>
@@ -3210,13 +3114,13 @@
         <v>428</v>
       </c>
       <c r="F7" t="n">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="G7" t="n">
         <v>99.689</v>
       </c>
       <c r="H7" t="n">
-        <v>353.988</v>
+        <v>355.776</v>
       </c>
       <c r="I7" t="n">
         <v>26.9</v>
@@ -3228,22 +3132,22 @@
         <v>643</v>
       </c>
       <c r="L7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="M7" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="N7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="O7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="P7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="Q7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="R7" t="n">
         <v>99.5</v>
@@ -3291,22 +3195,22 @@
         <v>53</v>
       </c>
       <c r="AK7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="AL7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AM7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="AN7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="AO7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="AP7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="AQ7" t="n">
         <v>98.6</v>
@@ -3327,41 +3231,29 @@
         <v>98.6</v>
       </c>
       <c r="AW7" t="n">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="AX7" t="n">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AY7" t="n">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="AZ7" t="n">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="BA7" t="n">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="BB7" t="n">
-        <v>213</v>
-      </c>
-      <c r="BC7" t="n">
         <v>210</v>
       </c>
-      <c r="BD7" t="n">
-        <v>212</v>
-      </c>
-      <c r="BE7" t="n">
-        <v>210</v>
-      </c>
-      <c r="BF7" t="n">
-        <v>210</v>
-      </c>
-      <c r="BG7" t="n">
-        <v>210</v>
-      </c>
-      <c r="BH7" t="n">
-        <v>210</v>
-      </c>
+      <c r="BC7"/>
+      <c r="BD7"/>
+      <c r="BE7"/>
+      <c r="BF7"/>
+      <c r="BG7"/>
+      <c r="BH7"/>
       <c r="BI7"/>
       <c r="BJ7"/>
       <c r="BK7"/>
@@ -3370,110 +3262,107 @@
       <c r="BN7"/>
       <c r="BO7"/>
       <c r="BP7"/>
-      <c r="BQ7"/>
-      <c r="BR7"/>
-      <c r="BS7"/>
-      <c r="BT7"/>
+      <c r="BQ7" t="s">
+        <v>60</v>
+      </c>
+      <c r="BR7" t="s">
+        <v>60</v>
+      </c>
+      <c r="BS7" t="s">
+        <v>60</v>
+      </c>
+      <c r="BT7" t="s">
+        <v>60</v>
+      </c>
       <c r="BU7"/>
       <c r="BV7"/>
-      <c r="BW7" t="s">
-        <v>60</v>
-      </c>
-      <c r="BX7" t="s">
-        <v>60</v>
-      </c>
-      <c r="BY7" t="s">
-        <v>60</v>
-      </c>
-      <c r="BZ7" t="s">
-        <v>60</v>
-      </c>
-      <c r="CA7"/>
+      <c r="BW7"/>
+      <c r="BX7"/>
+      <c r="BY7"/>
+      <c r="BZ7"/>
+      <c r="CA7" t="n">
+        <v>213</v>
+      </c>
       <c r="CB7"/>
       <c r="CC7"/>
-      <c r="CD7"/>
-      <c r="CE7"/>
-      <c r="CF7"/>
-      <c r="CG7"/>
-      <c r="CH7"/>
+      <c r="CD7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="CE7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="CF7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="CG7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="CH7" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="CI7" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="CJ7" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="CK7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="CL7" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="CM7" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="CN7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="CO7" t="n">
+      <c r="CJ7" t="n">
         <v>641</v>
       </c>
+      <c r="CK7" t="s">
+        <v>80</v>
+      </c>
+      <c r="CL7" t="s">
+        <v>176</v>
+      </c>
+      <c r="CM7" t="s">
+        <v>33</v>
+      </c>
+      <c r="CN7" t="s">
+        <v>26</v>
+      </c>
+      <c r="CO7" t="s">
+        <v>26</v>
+      </c>
       <c r="CP7" t="s">
-        <v>80</v>
-      </c>
-      <c r="CQ7" t="s">
-        <v>178</v>
-      </c>
-      <c r="CR7" t="s">
-        <v>33</v>
-      </c>
-      <c r="CS7" t="s">
-        <v>26</v>
-      </c>
-      <c r="CT7" t="s">
-        <v>26</v>
-      </c>
-      <c r="CU7" t="s">
         <v>68</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="CI2" r:id="rId1h"/>
-    <hyperlink ref="CJ2" r:id="rId2h"/>
-    <hyperlink ref="CK2" r:id="rId3h"/>
-    <hyperlink ref="CL2" r:id="rId4h"/>
-    <hyperlink ref="CM2" r:id="rId5h"/>
-    <hyperlink ref="CN2" r:id="rId6h"/>
-    <hyperlink ref="CI3" r:id="rId7h"/>
-    <hyperlink ref="CJ3" r:id="rId8h"/>
-    <hyperlink ref="CK3" r:id="rId9h"/>
-    <hyperlink ref="CL3" r:id="rId10h"/>
-    <hyperlink ref="CM3" r:id="rId11h"/>
-    <hyperlink ref="CN3" r:id="rId12h"/>
-    <hyperlink ref="CI4" r:id="rId13h"/>
-    <hyperlink ref="CJ4" r:id="rId14h"/>
-    <hyperlink ref="CK4" r:id="rId15h"/>
-    <hyperlink ref="CL4" r:id="rId16h"/>
-    <hyperlink ref="CM4" r:id="rId17h"/>
-    <hyperlink ref="CN4" r:id="rId18h"/>
-    <hyperlink ref="CI5" r:id="rId19h"/>
-    <hyperlink ref="CJ5" r:id="rId20h"/>
-    <hyperlink ref="CK5" r:id="rId21h"/>
-    <hyperlink ref="CL5" r:id="rId22h"/>
-    <hyperlink ref="CM5" r:id="rId23h"/>
-    <hyperlink ref="CN5" r:id="rId24h"/>
-    <hyperlink ref="CI6" r:id="rId25h"/>
-    <hyperlink ref="CJ6" r:id="rId26h"/>
-    <hyperlink ref="CK6" r:id="rId27h"/>
-    <hyperlink ref="CL6" r:id="rId28h"/>
-    <hyperlink ref="CM6" r:id="rId29h"/>
-    <hyperlink ref="CN6" r:id="rId30h"/>
-    <hyperlink ref="CI7" r:id="rId31h"/>
-    <hyperlink ref="CJ7" r:id="rId32h"/>
-    <hyperlink ref="CK7" r:id="rId33h"/>
-    <hyperlink ref="CL7" r:id="rId34h"/>
-    <hyperlink ref="CM7" r:id="rId35h"/>
-    <hyperlink ref="CN7" r:id="rId36h"/>
+    <hyperlink ref="CD2" r:id="rId1h"/>
+    <hyperlink ref="CE2" r:id="rId2h"/>
+    <hyperlink ref="CF2" r:id="rId3h"/>
+    <hyperlink ref="CG2" r:id="rId4h"/>
+    <hyperlink ref="CH2" r:id="rId5h"/>
+    <hyperlink ref="CI2" r:id="rId6h"/>
+    <hyperlink ref="CD3" r:id="rId7h"/>
+    <hyperlink ref="CE3" r:id="rId8h"/>
+    <hyperlink ref="CF3" r:id="rId9h"/>
+    <hyperlink ref="CG3" r:id="rId10h"/>
+    <hyperlink ref="CH3" r:id="rId11h"/>
+    <hyperlink ref="CI3" r:id="rId12h"/>
+    <hyperlink ref="CD4" r:id="rId13h"/>
+    <hyperlink ref="CE4" r:id="rId14h"/>
+    <hyperlink ref="CF4" r:id="rId15h"/>
+    <hyperlink ref="CG4" r:id="rId16h"/>
+    <hyperlink ref="CH4" r:id="rId17h"/>
+    <hyperlink ref="CI4" r:id="rId18h"/>
+    <hyperlink ref="CD5" r:id="rId19h"/>
+    <hyperlink ref="CE5" r:id="rId20h"/>
+    <hyperlink ref="CF5" r:id="rId21h"/>
+    <hyperlink ref="CG5" r:id="rId22h"/>
+    <hyperlink ref="CH5" r:id="rId23h"/>
+    <hyperlink ref="CI5" r:id="rId24h"/>
+    <hyperlink ref="CD6" r:id="rId25h"/>
+    <hyperlink ref="CE6" r:id="rId26h"/>
+    <hyperlink ref="CF6" r:id="rId27h"/>
+    <hyperlink ref="CG6" r:id="rId28h"/>
+    <hyperlink ref="CH6" r:id="rId29h"/>
+    <hyperlink ref="CI6" r:id="rId30h"/>
+    <hyperlink ref="CD7" r:id="rId31h"/>
+    <hyperlink ref="CE7" r:id="rId32h"/>
+    <hyperlink ref="CF7" r:id="rId33h"/>
+    <hyperlink ref="CG7" r:id="rId34h"/>
+    <hyperlink ref="CH7" r:id="rId35h"/>
+    <hyperlink ref="CI7" r:id="rId36h"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>